<commit_message>
Explored libuv and V8 Engine
- Working of async tasks in NodeJS using libuv
- Working of V8 Engine
- Working of Event Loop and it phases
</commit_message>
<xml_diff>
--- a/NodeJS/Notes/Node JS Todo.xlsx
+++ b/NodeJS/Notes/Node JS Todo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\SKILLS\Full Stack Devlopment\WEB DEV\Learning-Web-Devlopment-MERN-Stack\NodeJS\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D082C5CE-E342-455A-8E22-41AAB776B47B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C779455B-C796-4CE4-9510-EDFC9BEC5A48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{6852C7CF-E6FF-454A-9722-087CD06C98CB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6852C7CF-E6FF-454A-9722-087CD06C98CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,9 +37,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
-    <t>s-1</t>
-  </si>
-  <si>
     <t>Ep-0</t>
   </si>
   <si>
@@ -85,12 +82,6 @@
     <t>Ep-14</t>
   </si>
   <si>
-    <t>s-2</t>
-  </si>
-  <si>
-    <t>s-3</t>
-  </si>
-  <si>
     <t>S1-11 -&gt; S2 -2</t>
   </si>
   <si>
@@ -119,13 +110,22 @@
   </si>
   <si>
     <t>Goal</t>
+  </si>
+  <si>
+    <t>S-1</t>
+  </si>
+  <si>
+    <t>S-2</t>
+  </si>
+  <si>
+    <t>S-3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -145,8 +145,14 @@
       <name val="Trebuchet MS"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Trebuchet MS"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -191,7 +197,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -208,14 +220,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -226,7 +232,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="2" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -543,8 +562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14F31291-AEC1-4B90-9E99-33DBAF374F1D}">
   <dimension ref="A3:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,75 +573,75 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>27</v>
+      <c r="A3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="9">
+      <c r="A4" s="5">
         <v>45902</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>45903</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>45904</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>45905</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>45906</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="9">
-        <v>45903</v>
-      </c>
-      <c r="B5" s="10" t="s">
+    <row r="9" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>45907</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="9">
-        <v>45904</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="9">
-        <v>45905</v>
-      </c>
-      <c r="B7" s="10" t="s">
+    <row r="10" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>45908</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="9">
-        <v>45906</v>
-      </c>
-      <c r="B8" s="10" t="s">
+    <row r="11" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <v>45909</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="9">
-        <v>45907</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="9">
-        <v>45908</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="9">
-        <v>45909</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -635,209 +654,212 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85C94DCB-BB32-4D05-872A-FB961E556115}">
   <dimension ref="A2:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="7"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" s="8">
+        <v>12</v>
+      </c>
+      <c r="C3" s="9">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B4" s="8">
+        <v>42</v>
+      </c>
+      <c r="C4" s="9">
+        <v>52</v>
+      </c>
+      <c r="D4" s="10">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="8">
+        <v>45</v>
+      </c>
+      <c r="C5" s="9">
+        <v>57</v>
+      </c>
+      <c r="D5" s="10">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="8">
+        <v>42</v>
+      </c>
+      <c r="C6" s="11">
+        <v>65</v>
+      </c>
+      <c r="D6" s="12">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="8">
+        <v>56</v>
+      </c>
+      <c r="C7" s="11">
+        <v>67</v>
+      </c>
+      <c r="D7" s="12">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="8">
+        <v>88</v>
+      </c>
+      <c r="C8" s="11">
+        <v>86</v>
+      </c>
+      <c r="D8" s="12">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="8">
+        <v>96</v>
+      </c>
+      <c r="C9" s="11">
+        <v>65</v>
+      </c>
+      <c r="D9" s="12">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="8">
+        <v>60</v>
+      </c>
+      <c r="C10" s="11">
+        <v>92</v>
+      </c>
+      <c r="D10" s="12">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="8">
+        <v>80</v>
+      </c>
+      <c r="C11" s="13">
+        <v>85</v>
+      </c>
+      <c r="D11" s="14">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="12">
+        <v>102</v>
+      </c>
+      <c r="C12" s="13">
+        <v>50</v>
+      </c>
+      <c r="D12" s="14">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="12">
+        <v>84</v>
+      </c>
+      <c r="C13" s="13">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="9">
+        <v>87</v>
+      </c>
+      <c r="C14" s="13">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="3">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="11">
-        <v>42</v>
-      </c>
-      <c r="C4" s="3">
-        <v>52</v>
-      </c>
-      <c r="D4" s="5">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="11">
-        <v>45</v>
-      </c>
-      <c r="C5" s="3">
-        <v>57</v>
-      </c>
-      <c r="D5" s="5">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="11">
-        <v>42</v>
-      </c>
-      <c r="C6" s="4">
-        <v>65</v>
-      </c>
-      <c r="D6" s="2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="11">
-        <v>56</v>
-      </c>
-      <c r="C7" s="4">
-        <v>67</v>
-      </c>
-      <c r="D7" s="2">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1">
-        <v>88</v>
-      </c>
-      <c r="C8" s="4">
-        <v>86</v>
-      </c>
-      <c r="D8" s="2">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="1">
-        <v>96</v>
-      </c>
-      <c r="C9" s="4">
-        <v>65</v>
-      </c>
-      <c r="D9" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="2">
-        <v>60</v>
-      </c>
-      <c r="C10" s="4">
-        <v>92</v>
-      </c>
-      <c r="D10" s="2">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="2">
-        <v>80</v>
-      </c>
-      <c r="C11" s="1">
-        <v>85</v>
-      </c>
-      <c r="D11" s="6">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="2">
-        <v>102</v>
-      </c>
-      <c r="C12" s="1">
-        <v>50</v>
-      </c>
-      <c r="D12" s="6">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="2">
-        <v>84</v>
-      </c>
-      <c r="C13" s="1">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="3">
-        <v>87</v>
-      </c>
-      <c r="C14" s="1">
+      <c r="B15" s="9">
+        <v>73</v>
+      </c>
+      <c r="C15" s="10">
         <v>111</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="3">
-        <v>73</v>
-      </c>
-      <c r="C15" s="5">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="B16" s="9">
+        <v>90</v>
+      </c>
+      <c r="C16" s="10">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="3">
-        <v>90</v>
-      </c>
-      <c r="C16" s="5">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" s="5">
+      <c r="C17" s="10">
         <v>75</v>
       </c>
     </row>

</xml_diff>

<commit_message>
How the Web Works and Servers
- Created http server
</commit_message>
<xml_diff>
--- a/NodeJS/Notes/Node JS Todo.xlsx
+++ b/NodeJS/Notes/Node JS Todo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\SKILLS\Full Stack Devlopment\WEB DEV\Learning-Web-Devlopment-MERN-Stack\NodeJS\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A5B9748-8A42-4D06-83F7-E2A6AFC28FE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF485C78-EBED-4CC2-8D17-194A822DC5D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{6852C7CF-E6FF-454A-9722-087CD06C98CB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6852C7CF-E6FF-454A-9722-087CD06C98CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -152,7 +152,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -204,6 +204,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -220,7 +226,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -246,6 +252,12 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="2" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -562,8 +574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14F31291-AEC1-4B90-9E99-33DBAF374F1D}">
   <dimension ref="A3:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -589,10 +601,10 @@
       </c>
     </row>
     <row r="5" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
+      <c r="A5" s="15">
         <v>45903</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="16" t="s">
         <v>17</v>
       </c>
     </row>
@@ -654,8 +666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85C94DCB-BB32-4D05-872A-FB961E556115}">
   <dimension ref="A2:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -815,7 +827,7 @@
       <c r="A13" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="12">
+      <c r="B13" s="8">
         <v>84</v>
       </c>
       <c r="C13" s="13">

</xml_diff>

<commit_message>
Connected NodeJS to MongoDB
- Visualized Tick of libUV Event Loop
 - MongoClient
- connection pool and string
</commit_message>
<xml_diff>
--- a/NodeJS/Notes/Node JS Todo.xlsx
+++ b/NodeJS/Notes/Node JS Todo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\SKILLS\Full Stack Devlopment\WEB DEV\Learning-Web-Devlopment-MERN-Stack\NodeJS\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF485C78-EBED-4CC2-8D17-194A822DC5D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CFD5541-9793-4D5A-83BF-F93BD849E02F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6852C7CF-E6FF-454A-9722-087CD06C98CB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{6852C7CF-E6FF-454A-9722-087CD06C98CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Ep-0</t>
   </si>
@@ -82,30 +82,15 @@
     <t>Ep-14</t>
   </si>
   <si>
-    <t>S1-11 -&gt; S2 -2</t>
-  </si>
-  <si>
     <t>S1 0 -&gt; 6</t>
   </si>
   <si>
     <t>S1 7 -&gt; 10</t>
   </si>
   <si>
-    <t>S2 3 -&gt; 7</t>
-  </si>
-  <si>
     <t>S2 8 -&gt; 11</t>
   </si>
   <si>
-    <t>S2 12 -&gt;  S3 -2</t>
-  </si>
-  <si>
-    <t>S3 3-7</t>
-  </si>
-  <si>
-    <t>S3 8-9</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
@@ -119,6 +104,39 @@
   </si>
   <si>
     <t>S-3</t>
+  </si>
+  <si>
+    <t>S1-12 -&gt; S2 -3</t>
+  </si>
+  <si>
+    <t>S2 4 -&gt; 8</t>
+  </si>
+  <si>
+    <t>S2 9 -&gt; 12</t>
+  </si>
+  <si>
+    <t>Ep-15</t>
+  </si>
+  <si>
+    <t>Ep-16</t>
+  </si>
+  <si>
+    <t>Ep-17</t>
+  </si>
+  <si>
+    <t>Ep-18</t>
+  </si>
+  <si>
+    <t>Ep-19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S2 13-&gt; 17 </t>
+  </si>
+  <si>
+    <t>S2 18 -&gt; S3 5</t>
+  </si>
+  <si>
+    <t>S3 6 -&gt; 9</t>
   </si>
 </sst>
 </file>
@@ -152,7 +170,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -167,12 +185,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -185,18 +197,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -210,6 +210,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -226,7 +250,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -238,26 +262,30 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="14" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="2" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="14" fontId="2" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="2" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -572,89 +600,112 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14F31291-AEC1-4B90-9E99-33DBAF374F1D}">
-  <dimension ref="A3:B11"/>
+  <dimension ref="B3:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="33" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="33" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B4" s="5">
+        <v>45902</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B5" s="12">
+        <v>45903</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B6" s="14">
+        <v>45904</v>
+      </c>
+      <c r="C6" s="15"/>
+    </row>
+    <row r="7" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B7" s="14">
+        <v>45905</v>
+      </c>
+      <c r="C7" s="15"/>
+    </row>
+    <row r="8" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B8" s="3">
+        <v>45906</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="2" t="s">
+    </row>
+    <row r="9" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B9" s="3">
+        <v>45907</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="5">
-        <v>45902</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="15">
-        <v>45903</v>
-      </c>
-      <c r="B5" s="16" t="s">
+    <row r="10" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B10" s="3">
+        <v>45908</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
-        <v>45904</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="3">
-        <v>45905</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="3">
-        <v>45906</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="3">
-        <v>45907</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="3">
-        <v>45908</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="3">
+    <row r="11" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B11" s="3">
         <v>45909</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>22</v>
-      </c>
+      <c r="C11" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B12" s="3">
+        <v>45910</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B13" s="3">
+        <v>45911</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B14" s="3">
+        <v>45912</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B15" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -664,10 +715,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85C94DCB-BB32-4D05-872A-FB961E556115}">
-  <dimension ref="A2:D17"/>
+  <dimension ref="A2:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -677,13 +728,13 @@
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B2" s="7" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -707,7 +758,7 @@
       <c r="C4" s="9">
         <v>52</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="11">
         <v>60</v>
       </c>
     </row>
@@ -721,7 +772,7 @@
       <c r="C5" s="9">
         <v>57</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="11">
         <v>58</v>
       </c>
     </row>
@@ -732,10 +783,10 @@
       <c r="B6" s="8">
         <v>42</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="9">
         <v>65</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="11">
         <v>30</v>
       </c>
     </row>
@@ -746,10 +797,10 @@
       <c r="B7" s="8">
         <v>56</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="10">
         <v>67</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="11">
         <v>50</v>
       </c>
     </row>
@@ -760,10 +811,10 @@
       <c r="B8" s="8">
         <v>88</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="10">
         <v>86</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="11">
         <v>40</v>
       </c>
     </row>
@@ -774,10 +825,10 @@
       <c r="B9" s="8">
         <v>96</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="10">
         <v>65</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D9" s="17">
         <v>60</v>
       </c>
     </row>
@@ -788,10 +839,10 @@
       <c r="B10" s="8">
         <v>60</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C10" s="10">
         <v>92</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D10" s="17">
         <v>175</v>
       </c>
     </row>
@@ -802,10 +853,10 @@
       <c r="B11" s="8">
         <v>80</v>
       </c>
-      <c r="C11" s="13">
+      <c r="C11" s="10">
         <v>85</v>
       </c>
-      <c r="D11" s="14">
+      <c r="D11" s="17">
         <v>112</v>
       </c>
     </row>
@@ -816,10 +867,10 @@
       <c r="B12" s="8">
         <v>102</v>
       </c>
-      <c r="C12" s="13">
+      <c r="C12" s="11">
         <v>50</v>
       </c>
-      <c r="D12" s="14">
+      <c r="D12" s="18">
         <v>80</v>
       </c>
     </row>
@@ -830,7 +881,7 @@
       <c r="B13" s="8">
         <v>84</v>
       </c>
-      <c r="C13" s="13">
+      <c r="C13" s="11">
         <v>120</v>
       </c>
     </row>
@@ -838,10 +889,10 @@
       <c r="A14" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="9">
+      <c r="B14" s="8">
         <v>87</v>
       </c>
-      <c r="C14" s="13">
+      <c r="C14" s="11">
         <v>111</v>
       </c>
     </row>
@@ -849,10 +900,10 @@
       <c r="A15" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B15" s="8">
         <v>73</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C15" s="16">
         <v>111</v>
       </c>
     </row>
@@ -873,6 +924,46 @@
       </c>
       <c r="C17" s="10">
         <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="10">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="10">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="11">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Express Middleware and Error Handling
-next and err parameters
- middleware chaining
-execution flow of routes
</commit_message>
<xml_diff>
--- a/NodeJS/Notes/Node JS Todo.xlsx
+++ b/NodeJS/Notes/Node JS Todo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\SKILLS\Full Stack Devlopment\WEB DEV\Learning-Web-Devlopment-MERN-Stack\NodeJS\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A80E66E3-8196-404C-AC36-F6990CFBACBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82409272-5225-40AF-B539-D3E65A91067A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6852C7CF-E6FF-454A-9722-087CD06C98CB}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Ep-0</t>
   </si>
@@ -137,6 +137,9 @@
   </si>
   <si>
     <t>S3 6 -&gt; 9</t>
+  </si>
+  <si>
+    <t>A</t>
   </si>
 </sst>
 </file>
@@ -244,7 +247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -279,6 +282,12 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="2" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -593,10 +602,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14F31291-AEC1-4B90-9E99-33DBAF374F1D}">
-  <dimension ref="B3:C15"/>
+  <dimension ref="B3:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -605,7 +614,7 @@
     <col min="3" max="3" width="33" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>18</v>
       </c>
@@ -613,7 +622,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B4" s="5">
         <v>45902</v>
       </c>
@@ -621,7 +630,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B5" s="11">
         <v>45903</v>
       </c>
@@ -629,19 +638,19 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B6" s="13">
         <v>45904</v>
       </c>
       <c r="C6" s="14"/>
     </row>
-    <row r="7" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B7" s="13">
         <v>45905</v>
       </c>
       <c r="C7" s="14"/>
     </row>
-    <row r="8" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B8" s="11">
         <v>45906</v>
       </c>
@@ -649,7 +658,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B9" s="3">
         <v>45907</v>
       </c>
@@ -657,7 +666,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>45908</v>
       </c>
@@ -665,23 +674,26 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B11" s="3">
+    <row r="11" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B11" s="18">
         <v>45909</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="19" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
         <v>45910</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="13" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="J12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <v>45911</v>
       </c>
@@ -689,7 +701,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
         <v>45912</v>
       </c>
@@ -697,7 +709,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B15" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Validating API and Hashing Passwords
</commit_message>
<xml_diff>
--- a/NodeJS/Notes/Node JS Todo.xlsx
+++ b/NodeJS/Notes/Node JS Todo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\SKILLS\Full Stack Devlopment\WEB DEV\Learning-Web-Devlopment-MERN-Stack\NodeJS\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82409272-5225-40AF-B539-D3E65A91067A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{783CEB2E-EF47-4405-819E-2F556C6F8552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6852C7CF-E6FF-454A-9722-087CD06C98CB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{6852C7CF-E6FF-454A-9722-087CD06C98CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -604,7 +604,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14F31291-AEC1-4B90-9E99-33DBAF374F1D}">
   <dimension ref="B3:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -722,8 +722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85C94DCB-BB32-4D05-872A-FB961E556115}">
   <dimension ref="A2:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -802,7 +802,7 @@
       <c r="B7" s="8">
         <v>56</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="8">
         <v>67</v>
       </c>
       <c r="D7" s="10">
@@ -816,7 +816,7 @@
       <c r="B8" s="8">
         <v>88</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="8">
         <v>86</v>
       </c>
       <c r="D8" s="10">
@@ -830,7 +830,7 @@
       <c r="B9" s="8">
         <v>96</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="8">
         <v>65</v>
       </c>
       <c r="D9" s="16">
@@ -844,7 +844,7 @@
       <c r="B10" s="8">
         <v>60</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="8">
         <v>92</v>
       </c>
       <c r="D10" s="16">
@@ -858,7 +858,7 @@
       <c r="B11" s="8">
         <v>80</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="8">
         <v>85</v>
       </c>
       <c r="D11" s="16">
@@ -872,7 +872,7 @@
       <c r="B12" s="8">
         <v>102</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="8">
         <v>50</v>
       </c>
       <c r="D12" s="17">

</xml_diff>

<commit_message>
JWT Tokens , Auth Middleware ad Swagger Report
- created tokens and cookies
- created an auth middleware
- Generated Interactive API report using Swagger UI
</commit_message>
<xml_diff>
--- a/NodeJS/Notes/Node JS Todo.xlsx
+++ b/NodeJS/Notes/Node JS Todo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\SKILLS\Full Stack Devlopment\WEB DEV\Learning-Web-Devlopment-MERN-Stack\NodeJS\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{783CEB2E-EF47-4405-819E-2F556C6F8552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37B8030F-5209-4D10-93B2-457B77217953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{6852C7CF-E6FF-454A-9722-087CD06C98CB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6852C7CF-E6FF-454A-9722-087CD06C98CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Ep-0</t>
   </si>
@@ -136,10 +136,16 @@
     <t>S2 18 -&gt; S3 5</t>
   </si>
   <si>
-    <t>S3 6 -&gt; 9</t>
-  </si>
-  <si>
-    <t>A</t>
+    <t>S2 11 -&gt; 14</t>
+  </si>
+  <si>
+    <t>S2 15 -&gt; 19</t>
+  </si>
+  <si>
+    <t>S3 1 -&gt; 6</t>
+  </si>
+  <si>
+    <t>S3 7 -&gt; 9</t>
   </si>
 </sst>
 </file>
@@ -173,7 +179,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -188,12 +194,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -218,19 +218,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79998168889431442"/>
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
+        <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -247,7 +259,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -259,33 +271,36 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="14" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="2" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -602,10 +617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14F31291-AEC1-4B90-9E99-33DBAF374F1D}">
-  <dimension ref="B3:J15"/>
+  <dimension ref="B3:C17"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,7 +629,7 @@
     <col min="3" max="3" width="33" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>18</v>
       </c>
@@ -622,7 +637,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B4" s="5">
         <v>45902</v>
       </c>
@@ -630,87 +645,105 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B5" s="11">
+    <row r="5" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B5" s="10">
         <v>45903</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B6" s="13">
+    <row r="6" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B6" s="12">
         <v>45904</v>
       </c>
-      <c r="C6" s="14"/>
-    </row>
-    <row r="7" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B7" s="13">
+      <c r="C6" s="13"/>
+    </row>
+    <row r="7" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B7" s="12">
         <v>45905</v>
       </c>
-      <c r="C7" s="14"/>
-    </row>
-    <row r="8" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B8" s="11">
+      <c r="C7" s="13"/>
+    </row>
+    <row r="8" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B8" s="10">
         <v>45906</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="11" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B9" s="3">
+    <row r="9" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B9" s="12">
         <v>45907</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="18" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B10" s="3">
+    <row r="10" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B10" s="12">
         <v>45908</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B11" s="18">
+    <row r="11" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B11" s="12">
         <v>45909</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="18" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B12" s="3">
+    <row r="12" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B12" s="12">
         <v>45910</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="J12" t="s">
+    </row>
+    <row r="13" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B13" s="12">
+        <v>45911</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B14" s="19">
+        <v>45912</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B15" s="3">
+        <v>45913</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B13" s="3">
-        <v>45911</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B14" s="3">
-        <v>45912</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B15" s="3"/>
+    <row r="16" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B16" s="3">
+        <v>45914</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B17" s="3">
+        <v>45915</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>36</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -722,8 +755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85C94DCB-BB32-4D05-872A-FB961E556115}">
   <dimension ref="A2:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -763,7 +796,7 @@
       <c r="C4" s="8">
         <v>52</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="14">
         <v>60</v>
       </c>
     </row>
@@ -777,7 +810,7 @@
       <c r="C5" s="8">
         <v>57</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="14">
         <v>58</v>
       </c>
     </row>
@@ -791,7 +824,7 @@
       <c r="C6" s="8">
         <v>65</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="14">
         <v>30</v>
       </c>
     </row>
@@ -805,7 +838,7 @@
       <c r="C7" s="8">
         <v>67</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="14">
         <v>50</v>
       </c>
     </row>
@@ -819,7 +852,7 @@
       <c r="C8" s="8">
         <v>86</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="14">
         <v>40</v>
       </c>
     </row>
@@ -833,7 +866,7 @@
       <c r="C9" s="8">
         <v>65</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D9" s="14">
         <v>60</v>
       </c>
     </row>
@@ -847,7 +880,7 @@
       <c r="C10" s="8">
         <v>92</v>
       </c>
-      <c r="D10" s="16">
+      <c r="D10" s="17">
         <v>175</v>
       </c>
     </row>
@@ -861,7 +894,7 @@
       <c r="C11" s="8">
         <v>85</v>
       </c>
-      <c r="D11" s="16">
+      <c r="D11" s="17">
         <v>112</v>
       </c>
     </row>
@@ -886,7 +919,7 @@
       <c r="B13" s="8">
         <v>84</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="9">
         <v>120</v>
       </c>
     </row>
@@ -897,7 +930,7 @@
       <c r="B14" s="8">
         <v>87</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="15">
         <v>111</v>
       </c>
     </row>
@@ -919,7 +952,7 @@
       <c r="B16" s="8">
         <v>90</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C16" s="15">
         <v>82</v>
       </c>
     </row>
@@ -927,7 +960,7 @@
       <c r="A17" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="9">
+      <c r="C17" s="15">
         <v>75</v>
       </c>
     </row>
@@ -935,7 +968,7 @@
       <c r="A18" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="9">
+      <c r="C18" s="16">
         <v>80</v>
       </c>
     </row>
@@ -943,7 +976,7 @@
       <c r="A19" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C19" s="16">
         <v>90</v>
       </c>
     </row>
@@ -951,7 +984,7 @@
       <c r="A20" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="9">
+      <c r="C20" s="16">
         <v>104</v>
       </c>
     </row>
@@ -959,7 +992,7 @@
       <c r="A21" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="10">
+      <c r="C21" s="16">
         <v>70</v>
       </c>
     </row>
@@ -967,7 +1000,7 @@
       <c r="A22" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="10">
+      <c r="C22" s="16">
         <v>64</v>
       </c>
     </row>

</xml_diff>

<commit_message>
JS: every() and _id , __v
</commit_message>
<xml_diff>
--- a/NodeJS/Notes/Node JS Todo.xlsx
+++ b/NodeJS/Notes/Node JS Todo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\SKILLS\Full Stack Devlopment\WEB DEV\Learning-Web-Devlopment-MERN-Stack\NodeJS\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42C84D96-5994-4308-B128-488F1DFA1B70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D04316FE-0229-40C1-A8A5-1C2E5E4446A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{6852C7CF-E6FF-454A-9722-087CD06C98CB}"/>
   </bookViews>
@@ -179,7 +179,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -218,12 +218,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="3" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -253,7 +247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -286,14 +280,13 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -670,7 +663,7 @@
       <c r="B9" s="11">
         <v>45907</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="16" t="s">
         <v>24</v>
       </c>
     </row>
@@ -678,7 +671,7 @@
       <c r="B10" s="11">
         <v>45908</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="16" t="s">
         <v>17</v>
       </c>
     </row>
@@ -686,7 +679,7 @@
       <c r="B11" s="11">
         <v>45909</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="16" t="s">
         <v>25</v>
       </c>
     </row>
@@ -694,7 +687,7 @@
       <c r="B12" s="11">
         <v>45910</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="16" t="s">
         <v>31</v>
       </c>
     </row>
@@ -702,15 +695,15 @@
       <c r="B13" s="11">
         <v>45911</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="16" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="14" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B14" s="18">
+      <c r="B14" s="17">
         <v>45912</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="18" t="s">
         <v>33</v>
       </c>
     </row>
@@ -749,7 +742,7 @@
   <dimension ref="A2:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -873,7 +866,7 @@
       <c r="C10" s="8">
         <v>92</v>
       </c>
-      <c r="D10" s="16">
+      <c r="D10" s="15">
         <v>175</v>
       </c>
     </row>
@@ -887,7 +880,7 @@
       <c r="C11" s="8">
         <v>85</v>
       </c>
-      <c r="D11" s="16">
+      <c r="D11" s="15">
         <v>112</v>
       </c>
     </row>
@@ -901,7 +894,7 @@
       <c r="C12" s="8">
         <v>50</v>
       </c>
-      <c r="D12" s="16">
+      <c r="D12" s="15">
         <v>80</v>
       </c>
     </row>
@@ -953,7 +946,7 @@
       <c r="A17" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="14">
+      <c r="C17" s="8">
         <v>75</v>
       </c>
     </row>
@@ -961,7 +954,7 @@
       <c r="A18" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="15">
+      <c r="C18" s="14">
         <v>80</v>
       </c>
     </row>
@@ -969,7 +962,7 @@
       <c r="A19" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="15">
+      <c r="C19" s="14">
         <v>90</v>
       </c>
     </row>
@@ -977,7 +970,7 @@
       <c r="A20" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="15">
+      <c r="C20" s="14">
         <v>104</v>
       </c>
     </row>
@@ -985,7 +978,7 @@
       <c r="A21" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="15">
+      <c r="C21" s="14">
         <v>70</v>
       </c>
     </row>
@@ -993,7 +986,7 @@
       <c r="A22" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="15">
+      <c r="C22" s="14">
         <v>64</v>
       </c>
     </row>

</xml_diff>